<commit_message>
PROS-5232 - CCRU - KPI update 10.06 - Change logical operator for "Drink out: Morning coffee" from "AND" to "OR".
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/HoReCa Cofee_Tea Shops PoS 2018.xlsx
+++ b/Projects/CCRU/Data/HoReCa Cofee_Tea Shops PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="HoReCa Cofee_Tea Shops" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,6 +36,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Cofee_Tea Shops'!$B$1:$AP$38</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Cofee_Tea Shops'!$B$1:$AP$38</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Cofee_Tea Shops'!$B$1:$AP$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'HoReCa Cofee_Tea Shops'!$B$1:$AP$38</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -62,7 +63,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 comments</t>
         </r>
       </text>
@@ -77,7 +78,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -92,7 +93,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -107,7 +108,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Aleksandra Danilenko:
+          <t xml:space="preserve">Aleksandra Danilenko:
 sku или сцена??</t>
         </r>
       </text>
@@ -117,596 +118,593 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="191">
-  <si>
-    <t>Sorting</t>
-  </si>
-  <si>
-    <t>SAP PoS</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>KPI Type</t>
-  </si>
-  <si>
-    <t>SAP KPI</t>
-  </si>
-  <si>
-    <t>KPI name Eng</t>
-  </si>
-  <si>
-    <t>KPI name Rus</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>target_min</t>
-  </si>
-  <si>
-    <t>target_max</t>
-  </si>
-  <si>
-    <t>SKU</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>Product Category</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Logical Operator</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Form Factor</t>
-  </si>
-  <si>
-    <t>Zone to include</t>
-  </si>
-  <si>
-    <t>Locations to exclude</t>
-  </si>
-  <si>
-    <t>Locations to include</t>
-  </si>
-  <si>
-    <t>Scenes to include</t>
-  </si>
-  <si>
-    <t>Scenes to exclude</t>
-  </si>
-  <si>
-    <t>sub locations to include</t>
-  </si>
-  <si>
-    <t>sub locations to exclude</t>
-  </si>
-  <si>
-    <t>Converted?</t>
-  </si>
-  <si>
-    <t>score_func</t>
-  </si>
-  <si>
-    <t>KPI Weight</t>
-  </si>
-  <si>
-    <t>score_min</t>
-  </si>
-  <si>
-    <t>score_max</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Base KPI for TOP 5 GAPs</t>
-  </si>
-  <si>
-    <t>KPI from POS 2016</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>KPI ID</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>To include in first calculation?</t>
-  </si>
-  <si>
-    <t>Target Execution 2018</t>
-  </si>
-  <si>
-    <t>RD38010007</t>
-  </si>
-  <si>
-    <t>HoReCa (Cofee /Tea Shops)</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>STANDARD 1</t>
-  </si>
-  <si>
-    <t>SSD Availability</t>
-  </si>
-  <si>
-    <t>Представленность SSD</t>
-  </si>
-  <si>
-    <t>Weighted Average </t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="190">
+  <si>
+    <t xml:space="preserve">Sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP PoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Rus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_func</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base KPI for TOP 5 GAPs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI from POS 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To include in first calculation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target Execution 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD38010007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoReCa (Cofee /Tea Shops)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Average </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2
 3
 4
 5</t>
   </si>
   <si>
-    <t>Coca-Cola - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>number of facings</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>SKUs</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Panoramic Photo</t>
-  </si>
-  <si>
-    <t>BINARY</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>Sprite - 0.25L Glass</t>
-  </si>
-  <si>
-    <t>Спрайт - 0.25л стекло</t>
-  </si>
-  <si>
-    <t>Schweppes Tonic - 0.25L Glass</t>
-  </si>
-  <si>
-    <t>Швеппс Тоник - 0.25л стекло</t>
-  </si>
-  <si>
-    <t>STANDARD 2</t>
-  </si>
-  <si>
-    <t>Water Availability</t>
-  </si>
-  <si>
-    <t>Представленность Воды</t>
-  </si>
-  <si>
-    <t>7
+    <t xml:space="preserve">Coca-Cola - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panoramic Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.25L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.25л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 0.25L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 0.25л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Воды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7
 8
 9</t>
   </si>
   <si>
-    <t>BonAqua Still - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>BonAqua Carb - 0.33L Glass</t>
-  </si>
-  <si>
-    <t>БонАква Газ - 0.33л стекло</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 0.75L Glass</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 0.75л стекло</t>
-  </si>
-  <si>
-    <t>Juice Availability</t>
-  </si>
-  <si>
-    <t>Представленность Сока</t>
-  </si>
-  <si>
-    <t>11
+    <t xml:space="preserve">BonAqua Still - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Carb - 0.33L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Газ - 0.33л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.75L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.75л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Сока</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11
 12
 13</t>
   </si>
   <si>
-    <t>Rich - Orange - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Апельсин - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich - Apple - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Яблоко - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Rich - Cherry - 0.2L Glass</t>
-  </si>
-  <si>
-    <t>Рич - Вишня - 0.2л стекло</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>LOCAL 3</t>
-  </si>
-  <si>
-    <t>Spirits Availability</t>
-  </si>
-  <si>
-    <t>Представленность Алкоголя</t>
-  </si>
-  <si>
-    <t>Weighted Average</t>
-  </si>
-  <si>
-    <t>15
+    <t xml:space="preserve">Rich - Orange - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Апельсин - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Apple - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Яблоко - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Cherry - 0.2L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Вишня - 0.2л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCAL 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirits Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Алкоголя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15
 16
 17</t>
   </si>
   <si>
-    <t>Red Hackle - 0.7L</t>
-  </si>
-  <si>
-    <t>Рэд Хакл - 0.7л</t>
-  </si>
-  <si>
-    <t>Wild Turkey 81 - 0.7L</t>
-  </si>
-  <si>
-    <t>Уайлд Тёки 81 - 0.7л</t>
-  </si>
-  <si>
-    <t>New Alco Brand</t>
-  </si>
-  <si>
-    <t>not defined</t>
-  </si>
-  <si>
-    <t>STANDARD 16</t>
-  </si>
-  <si>
-    <t>Menu Activation</t>
-  </si>
-  <si>
-    <t>Активация Меню</t>
-  </si>
-  <si>
-    <t>Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle</t>
-  </si>
-  <si>
-    <t>5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004</t>
-  </si>
-  <si>
-    <t>Activation</t>
-  </si>
-  <si>
-    <t>Other Menu Activation, Menu, Menu Insert</t>
-  </si>
-  <si>
-    <t>STANDARD 17</t>
-  </si>
-  <si>
-    <t>Impulse Activation</t>
-  </si>
-  <si>
-    <t>Активация Импульсной зоны</t>
-  </si>
-  <si>
-    <t>number of atomic KPI Passed</t>
-  </si>
-  <si>
-    <t>Bar Activation</t>
-  </si>
-  <si>
-    <t>20
+    <t xml:space="preserve">Red Hackle - 0.7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рэд Хакл - 0.7л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wild Turkey 81 - 0.7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Уайлд Тёки 81 - 0.7л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Alco Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not defined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Меню</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Menu Activation, Menu, Menu Insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Импульсной зоны</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of atomic KPI Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20
 21
 22</t>
   </si>
   <si>
-    <t>Impulse: SSD/Water/Juice NRGB</t>
-  </si>
-  <si>
-    <t>Импульс: SSD/Water/Juice Стекло</t>
-  </si>
-  <si>
-    <t>Manufacture: TCCC</t>
-  </si>
-  <si>
-    <t>SSD, Water, Juices</t>
-  </si>
-  <si>
-    <t>MAN in CAT</t>
-  </si>
-  <si>
-    <t>glass</t>
-  </si>
-  <si>
-    <t>Impulse: Burn CAN</t>
-  </si>
-  <si>
-    <t>Импульс: Burn Банка</t>
-  </si>
-  <si>
-    <t>Burn</t>
-  </si>
-  <si>
-    <t>BRAND</t>
-  </si>
-  <si>
-    <t>CAN, can</t>
-  </si>
-  <si>
-    <t>Impulse: Alcohol</t>
-  </si>
-  <si>
-    <t>Импульс: Замиксуй (Дисплей Алкоголя)</t>
-  </si>
-  <si>
-    <t>number of SKUs</t>
-  </si>
-  <si>
-    <t>Manufacture: TCCC, CAMPARI</t>
-  </si>
-  <si>
-    <t>Spirits</t>
-  </si>
-  <si>
-    <t>TCCC, CAMPARI</t>
-  </si>
-  <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>Destination Activation</t>
-  </si>
-  <si>
-    <t>Активация Стола</t>
-  </si>
-  <si>
-    <t>Table Activation</t>
-  </si>
-  <si>
-    <t>24
+    <t xml:space="preserve">Impulse: SSD/Water/Juice NRGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Импульс: SSD/Water/Juice Стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture: TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD, Water, Juices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN in CAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse: Burn CAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Импульс: Burn Банка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN, can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse: Alcohol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Импульс: Замиксуй (Дисплей Алкоголя)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture: TCCC, CAMPARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCC, CAMPARI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Стола</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24
 25</t>
   </si>
   <si>
-    <t>Destination: Images</t>
-  </si>
-  <si>
-    <t>Активация Стола: Имиджи</t>
-  </si>
-  <si>
-    <t>IC Activation</t>
-  </si>
-  <si>
-    <t>Destination: Coca-Cola/Bon Aqua NRGB</t>
-  </si>
-  <si>
-    <t>Активация Стола: Coca-Cola/Bon Aqua NRGB</t>
-  </si>
-  <si>
-    <t>Coca-Cola, Bonaqua</t>
-  </si>
-  <si>
-    <t>OCCASIONS</t>
-  </si>
-  <si>
-    <t>Drink Out: Morning coffee</t>
-  </si>
-  <si>
-    <t>Повод: Завтрак/утренний кофе</t>
-  </si>
-  <si>
-    <t>AND</t>
-  </si>
-  <si>
-    <t>Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
-  </si>
-  <si>
-    <t>27
+    <t xml:space="preserve">Destination: Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Стола: Имиджи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination: Coca-Cola/Bon Aqua NRGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Стола: Coca-Cola/Bon Aqua NRGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola, Bonaqua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCCASIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drink Out: Morning coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Повод: Завтрак/утренний кофе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27
 28</t>
   </si>
   <si>
-    <t>Morning coffee: BonAqua NRGB Image</t>
-  </si>
-  <si>
-    <t>Завтрак/утренний кофе: Бонаква Стекло Имидж</t>
-  </si>
-  <si>
-    <t>Sub Category: Glass</t>
-  </si>
-  <si>
-    <t>Glass</t>
-  </si>
-  <si>
-    <t>Bonaqua</t>
-  </si>
-  <si>
-    <t>SUB_CATEGORY</t>
-  </si>
-  <si>
-    <t>Morning coffee: BonAqua NRGB Product</t>
-  </si>
-  <si>
-    <t>Завтрак/утренний кофе: Бонаква Стекло Продукт</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Drink Out: Midday socializing</t>
-  </si>
-  <si>
-    <t>Повод: Relax после работы</t>
-  </si>
-  <si>
-    <t>30
+    <t xml:space="preserve">Morning coffee: BonAqua NRGB Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завтрак/утренний кофе: Бонаква Стекло Имидж</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Category: Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonaqua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB_CATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning coffee: BonAqua NRGB Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Завтрак/утренний кофе: Бонаква Стекло Продукт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drink Out: Midday socializing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Повод: Relax после работы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30
 31</t>
   </si>
   <si>
-    <t>Midday socializing: Mixability</t>
-  </si>
-  <si>
-    <t>Relax после работы: Миксабилити</t>
-  </si>
-  <si>
-    <t>RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry</t>
-  </si>
-  <si>
-    <t>A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002</t>
-  </si>
-  <si>
-    <t>Midday socializing: Moctails</t>
-  </si>
-  <si>
-    <t>Relax после работы: Моктели</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>Eat Out: Informal lunch</t>
-  </si>
-  <si>
-    <t>Повод: Ужин</t>
-  </si>
-  <si>
-    <t>Rich</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Visible Cooler</t>
-  </si>
-  <si>
-    <t>Видимый ХО</t>
-  </si>
-  <si>
-    <t>Cooler</t>
-  </si>
-  <si>
-    <t>34
+    <t xml:space="preserve">Midday socializing: Mixability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relax после работы: Миксабилити</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RED Hackle mix_img (2), Finlandia and Rich Cherry, Finlandia and Rich menu insert, Finlandia and Rich Mix, Finlandia and Rich Orange, Finlandia and Rich table tent, Finlandia and Schweppes Menu Insert, Finlandia and Schweppes Table Tent, Finlandia and Schweppes, Jack and Coke Menu, Jack and Coke Table tent, Jack Daniles and Coke Mix, Jack Daniles and Coke, Finlandia and Rich Sticker Cherry, Finlandia and Rich Sticker Orange, Finlandia and Rich table tent Cherry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5B10100, A5B10101, 7777888899, 7777888900, 7777888901, 7777888902, 7777888903, 7777888904, 7777888905, 7777888906, 7777888907, 7777888908, 7777888909, 7777888910, 7777889000, 7777889001, 7777889002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midday socializing: Moctails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relax после работы: Моктели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eat Out: Informal lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Повод: Ужин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Видимый ХО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34
 35
 36
 37</t>
   </si>
   <si>
-    <t>Cooler is Visible</t>
-  </si>
-  <si>
-    <t>ХО виден</t>
-  </si>
-  <si>
-    <t>Scenes with no tagging</t>
-  </si>
-  <si>
-    <t>SCENES</t>
-  </si>
-  <si>
-    <t>Panoramic photo of Cooler</t>
-  </si>
-  <si>
-    <t>Cooler fullness</t>
-  </si>
-  <si>
-    <t>ХО Заполнен</t>
-  </si>
-  <si>
-    <t>number of filled Coolers (scenes)</t>
-  </si>
-  <si>
-    <t>TCCC</t>
-  </si>
-  <si>
-    <t>MAN</t>
-  </si>
-  <si>
-    <t>SOS with empty more than 80%</t>
-  </si>
-  <si>
-    <t>Cooler wo other products</t>
-  </si>
-  <si>
-    <t>ХО без посторонней продукции</t>
-  </si>
-  <si>
-    <t>number of pure Coolers</t>
-  </si>
-  <si>
-    <t>Share of TCCC product at least 98%</t>
-  </si>
-  <si>
-    <t>Cooler: Max 14</t>
-  </si>
-  <si>
-    <t>Холодильники: Максимум 12 СКЮ на дверь</t>
-  </si>
-  <si>
-    <t>number of SKU per Door RANGE</t>
-  </si>
-  <si>
-    <t>Scene</t>
-  </si>
-  <si>
-    <t>KPI Score Formula</t>
-  </si>
-  <si>
-    <t>KPI weighted Score</t>
-  </si>
-  <si>
-    <t>Will be added on the 16th of December</t>
+    <t xml:space="preserve">Cooler is Visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО виден</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes with no tagging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCENES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panoramic photo of Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler fullness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО Заполнен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of filled Coolers (scenes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS with empty more than 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler wo other products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ХО без посторонней продукции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of pure Coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of TCCC product at least 98%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Max 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Максимум 12 СКЮ на дверь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of SKU per Door RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Score Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI weighted Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be added on the 16th of December</t>
   </si>
 </sst>
 </file>
@@ -714,7 +712,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
@@ -1374,9 +1372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1949400</xdr:colOff>
+      <xdr:colOff>1949040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1386,7 +1384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="14339520" cy="8909280"/>
+          <a:ext cx="14691600" cy="8908920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1419,9 +1417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1949400</xdr:colOff>
+      <xdr:colOff>1949040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1431,7 +1429,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="14339520" cy="8909280"/>
+          <a:ext cx="14691600" cy="8908920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1464,9 +1462,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1949400</xdr:colOff>
+      <xdr:colOff>1949040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1476,7 +1474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="14339520" cy="8909280"/>
+          <a:ext cx="14691600" cy="8908920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1509,9 +1507,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1949400</xdr:colOff>
+      <xdr:colOff>1949040</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1521,7 +1519,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="459000" y="0"/>
-          <a:ext cx="14339520" cy="8909280"/>
+          <a:ext cx="14691600" cy="8908920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1557,48 +1555,48 @@
   <dimension ref="A1:AP38"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="H2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="H18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="73.0976744186047"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.1627906976744"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="40.4883720930233"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="19" min="17" style="1" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="28.9209302325581"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="27" min="25" style="1" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="3" width="20.7953488372093"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="34.4558139534884"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="4" width="62.3906976744186"/>
-    <col collapsed="false" hidden="false" max="37" min="35" style="4" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.5813953488372"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="28.9209302325581"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="75.3162790697674"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.1488372093023"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="41.7162790697674"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="19" min="17" style="1" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="29.6558139534884"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="27" min="25" style="1" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="3" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="4" width="64.2372093023256"/>
+    <col collapsed="false" hidden="false" max="37" min="35" style="4" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="1" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="1" width="29.6558139534884"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3859,7 @@
       <c r="O27" s="34"/>
       <c r="P27" s="34"/>
       <c r="Q27" s="34" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="R27" s="34"/>
       <c r="S27" s="34"/>
@@ -3872,7 +3870,7 @@
         <v>100</v>
       </c>
       <c r="X27" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y27" s="34"/>
       <c r="Z27" s="34"/>
@@ -3899,7 +3897,7 @@
         <v>26</v>
       </c>
       <c r="AM27" s="73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AN27" s="36"/>
       <c r="AO27" s="36"/>
@@ -3924,10 +3922,10 @@
         <v>136</v>
       </c>
       <c r="F28" s="69" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" s="44" t="s">
         <v>142</v>
-      </c>
-      <c r="G28" s="44" t="s">
-        <v>143</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>52</v>
@@ -3938,23 +3936,23 @@
       <c r="J28" s="35"/>
       <c r="K28" s="35"/>
       <c r="L28" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="M28" s="34" t="s">
         <v>144</v>
-      </c>
-      <c r="M28" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="N28" s="34" t="s">
         <v>132</v>
       </c>
       <c r="O28" s="34"/>
       <c r="P28" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q28" s="34" t="s">
         <v>53</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
@@ -3964,7 +3962,7 @@
         <v>100</v>
       </c>
       <c r="X28" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y28" s="34"/>
       <c r="Z28" s="34"/>
@@ -4014,10 +4012,10 @@
         <v>136</v>
       </c>
       <c r="F29" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>148</v>
-      </c>
-      <c r="G29" s="44" t="s">
-        <v>149</v>
       </c>
       <c r="H29" s="34" t="s">
         <v>52</v>
@@ -4030,11 +4028,11 @@
       <c r="L29" s="34"/>
       <c r="M29" s="34"/>
       <c r="N29" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O29" s="34"/>
       <c r="P29" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q29" s="34" t="s">
         <v>53</v>
@@ -4102,10 +4100,10 @@
         <v>136</v>
       </c>
       <c r="F30" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="44" t="s">
         <v>151</v>
-      </c>
-      <c r="G30" s="44" t="s">
-        <v>152</v>
       </c>
       <c r="H30" s="34" t="s">
         <v>105</v>
@@ -4132,7 +4130,7 @@
         <v>100</v>
       </c>
       <c r="X30" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y30" s="34"/>
       <c r="Z30" s="34"/>
@@ -4159,7 +4157,7 @@
         <v>29</v>
       </c>
       <c r="AM30" s="73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AN30" s="36"/>
       <c r="AO30" s="36"/>
@@ -4184,10 +4182,10 @@
         <v>136</v>
       </c>
       <c r="F31" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="G31" s="44" t="s">
         <v>154</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>155</v>
       </c>
       <c r="H31" s="34" t="s">
         <v>52</v>
@@ -4198,10 +4196,10 @@
       <c r="J31" s="35"/>
       <c r="K31" s="35"/>
       <c r="L31" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="M31" s="78" t="s">
         <v>156</v>
-      </c>
-      <c r="M31" s="78" t="s">
-        <v>157</v>
       </c>
       <c r="N31" s="34"/>
       <c r="O31" s="34" t="s">
@@ -4222,7 +4220,7 @@
         <v>100</v>
       </c>
       <c r="X31" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y31" s="34"/>
       <c r="Z31" s="34"/>
@@ -4250,7 +4248,7 @@
       </c>
       <c r="AM31" s="36"/>
       <c r="AN31" s="69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AO31" s="36"/>
       <c r="AP31" s="28"/>
@@ -4272,10 +4270,10 @@
         <v>136</v>
       </c>
       <c r="F32" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="G32" s="44" t="s">
         <v>158</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>159</v>
       </c>
       <c r="H32" s="34" t="s">
         <v>52</v>
@@ -4286,10 +4284,10 @@
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
       <c r="L32" s="77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M32" s="77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N32" s="34"/>
       <c r="O32" s="34" t="s">
@@ -4310,7 +4308,7 @@
         <v>100</v>
       </c>
       <c r="X32" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y32" s="34"/>
       <c r="Z32" s="34"/>
@@ -4338,7 +4336,7 @@
       </c>
       <c r="AM32" s="36"/>
       <c r="AN32" s="69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AO32" s="36"/>
       <c r="AP32" s="28"/>
@@ -4360,10 +4358,10 @@
         <v>136</v>
       </c>
       <c r="F33" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="44" t="s">
         <v>161</v>
-      </c>
-      <c r="G33" s="44" t="s">
-        <v>162</v>
       </c>
       <c r="H33" s="34" t="s">
         <v>52</v>
@@ -4374,23 +4372,23 @@
       <c r="J33" s="35"/>
       <c r="K33" s="35"/>
       <c r="L33" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="M33" s="34" t="s">
         <v>144</v>
-      </c>
-      <c r="M33" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="N33" s="34" t="s">
         <v>132</v>
       </c>
       <c r="O33" s="34"/>
       <c r="P33" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q33" s="34" t="s">
         <v>53</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S33" s="34"/>
       <c r="T33" s="34"/>
@@ -4400,7 +4398,7 @@
         <v>100</v>
       </c>
       <c r="X33" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y33" s="34"/>
       <c r="Z33" s="34"/>
@@ -4447,13 +4445,13 @@
         <v>83</v>
       </c>
       <c r="E34" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="69" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="69" t="s">
+      <c r="G34" s="69" t="s">
         <v>165</v>
-      </c>
-      <c r="G34" s="69" t="s">
-        <v>166</v>
       </c>
       <c r="H34" s="75" t="s">
         <v>105</v>
@@ -4475,7 +4473,7 @@
       <c r="U34" s="34"/>
       <c r="V34" s="34"/>
       <c r="W34" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X34" s="34"/>
       <c r="Y34" s="34"/>
@@ -4503,7 +4501,7 @@
         <v>33</v>
       </c>
       <c r="AM34" s="73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AN34" s="0"/>
       <c r="AO34" s="36"/>
@@ -4523,16 +4521,16 @@
         <v>83</v>
       </c>
       <c r="E35" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F35" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="G35" s="74" t="s">
+      <c r="H35" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="I35" s="80" t="n">
         <v>1</v>
@@ -4548,7 +4546,7 @@
         <v>53</v>
       </c>
       <c r="R35" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S35" s="34"/>
       <c r="T35" s="34"/>
@@ -4558,7 +4556,7 @@
         <v>55</v>
       </c>
       <c r="X35" s="81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y35" s="34"/>
       <c r="Z35" s="34"/>
@@ -4586,7 +4584,7 @@
       </c>
       <c r="AM35" s="36"/>
       <c r="AN35" s="69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO35" s="36"/>
       <c r="AP35" s="28"/>
@@ -4605,16 +4603,16 @@
         <v>83</v>
       </c>
       <c r="E36" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F36" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="G36" s="74" t="s">
+      <c r="H36" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="I36" s="35" t="n">
         <v>1</v>
@@ -4625,7 +4623,7 @@
         <v>110</v>
       </c>
       <c r="M36" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N36" s="34"/>
       <c r="O36" s="34"/>
@@ -4634,14 +4632,14 @@
         <v>53</v>
       </c>
       <c r="R36" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S36" s="34"/>
       <c r="T36" s="34"/>
       <c r="U36" s="34"/>
       <c r="V36" s="34"/>
       <c r="W36" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X36" s="34"/>
       <c r="Y36" s="34"/>
@@ -4660,7 +4658,7 @@
       <c r="AF36" s="34"/>
       <c r="AG36" s="34"/>
       <c r="AH36" s="82" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AI36" s="35"/>
       <c r="AJ36" s="35"/>
@@ -4672,7 +4670,7 @@
       </c>
       <c r="AM36" s="36"/>
       <c r="AN36" s="69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO36" s="36"/>
       <c r="AP36" s="28"/>
@@ -4691,16 +4689,16 @@
         <v>83</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F37" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="G37" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="G37" s="74" t="s">
+      <c r="H37" s="34" t="s">
         <v>181</v>
-      </c>
-      <c r="H37" s="34" t="s">
-        <v>182</v>
       </c>
       <c r="I37" s="35" t="n">
         <v>1</v>
@@ -4711,7 +4709,7 @@
         <v>110</v>
       </c>
       <c r="M37" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N37" s="34"/>
       <c r="O37" s="34"/>
@@ -4720,14 +4718,14 @@
         <v>53</v>
       </c>
       <c r="R37" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="S37" s="34"/>
       <c r="T37" s="34"/>
       <c r="U37" s="34"/>
       <c r="V37" s="34"/>
       <c r="W37" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X37" s="34"/>
       <c r="Y37" s="34"/>
@@ -4746,7 +4744,7 @@
       <c r="AF37" s="34"/>
       <c r="AG37" s="34"/>
       <c r="AH37" s="82" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AI37" s="35"/>
       <c r="AJ37" s="35"/>
@@ -4758,7 +4756,7 @@
       </c>
       <c r="AM37" s="36"/>
       <c r="AN37" s="69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO37" s="36"/>
       <c r="AP37" s="28"/>
@@ -4778,13 +4776,13 @@
       </c>
       <c r="E38" s="58"/>
       <c r="F38" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="G38" s="44" t="s">
+      <c r="H38" s="83" t="s">
         <v>185</v>
-      </c>
-      <c r="H38" s="83" t="s">
-        <v>186</v>
       </c>
       <c r="I38" s="80"/>
       <c r="J38" s="80" t="n">
@@ -4797,7 +4795,7 @@
         <v>110</v>
       </c>
       <c r="M38" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N38" s="65"/>
       <c r="O38" s="65"/>
@@ -4813,7 +4811,7 @@
       <c r="U38" s="35"/>
       <c r="V38" s="35"/>
       <c r="W38" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X38" s="35"/>
       <c r="Y38" s="35"/>
@@ -4842,7 +4840,7 @@
       </c>
       <c r="AM38" s="36"/>
       <c r="AN38" s="69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AO38" s="36"/>
       <c r="AP38" s="28"/>
@@ -4874,7 +4872,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,10 +4895,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="86" t="s">
         <v>187</v>
-      </c>
-      <c r="H1" s="86" t="s">
-        <v>188</v>
       </c>
       <c r="I1" s="86" t="s">
         <v>32</v>
@@ -4909,7 +4907,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L1" s="86" t="s">
         <v>33</v>
@@ -4920,7 +4918,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="87" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>